<commit_message>
update id object def page
</commit_message>
<xml_diff>
--- a/docs/_sources/id_schema/Sample_ID_Object_Definition.xlsx
+++ b/docs/_sources/id_schema/Sample_ID_Object_Definition.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1045452\Documents\GitHub\documentation\docs\_sources\id_schema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91185303-983F-4BBC-9DDB-CE91291DF4F2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E43F2C0-3653-4B64-8BE4-B486899B2A1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Phase 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Phase 2" sheetId="3" r:id="rId2"/>
+    <sheet name="ID Schema" sheetId="1" r:id="rId1"/>
+    <sheet name="Registration Client UI Spec" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017"/>
 </workbook>
@@ -675,29 +675,32 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -711,17 +714,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -947,10 +947,10 @@
   <dimension ref="B2:O951"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="I4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A16" sqref="A16"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -974,66 +974,66 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="23" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="31" t="s">
         <v>127</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="31"/>
-      <c r="G2" s="36" t="s">
+      <c r="F2" s="32"/>
+      <c r="G2" s="34" t="s">
         <v>131</v>
       </c>
       <c r="H2" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="I2" s="31" t="s">
+      <c r="I2" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="29" t="s">
+      <c r="J2" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="K2" s="29" t="s">
+      <c r="K2" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="L2" s="29" t="s">
+      <c r="L2" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="M2" s="21" t="s">
+      <c r="M2" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="N2" s="21" t="s">
+      <c r="N2" s="23" t="s">
         <v>156</v>
       </c>
-      <c r="O2" s="21" t="s">
+      <c r="O2" s="23" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="3" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
       <c r="E3" s="17" t="s">
         <v>20</v>
       </c>
       <c r="F3" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="36"/>
+      <c r="G3" s="34"/>
       <c r="H3" s="38"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
     </row>
     <row r="4" spans="2:15" ht="28" x14ac:dyDescent="0.3">
       <c r="B4" s="11">
@@ -1116,25 +1116,25 @@
       <c r="O5" s="13"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B6" s="27">
+      <c r="B6" s="22">
         <v>3</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="32" t="s">
+      <c r="F6" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="27" t="s">
+      <c r="G6" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="H6" s="33" t="s">
+      <c r="H6" s="27" t="s">
         <v>5</v>
       </c>
       <c r="I6" s="11" t="s">
@@ -1143,10 +1143,10 @@
       <c r="J6" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K6" s="27" t="s">
+      <c r="K6" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="L6" s="27" t="s">
+      <c r="L6" s="22" t="s">
         <v>109</v>
       </c>
       <c r="M6" s="24"/>
@@ -1154,45 +1154,45 @@
       <c r="O6" s="13"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B7" s="27"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="35"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="28"/>
       <c r="I7" s="11" t="s">
         <v>6</v>
       </c>
       <c r="J7" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
-      <c r="M7" s="26"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="25"/>
       <c r="N7" s="8"/>
       <c r="O7" s="13"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B8" s="27">
+      <c r="B8" s="22">
         <v>4</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="32" t="s">
+      <c r="F8" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="G8" s="27" t="s">
+      <c r="G8" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="H8" s="33" t="s">
+      <c r="H8" s="27" t="s">
         <v>5</v>
       </c>
       <c r="I8" s="11" t="s">
@@ -1201,10 +1201,10 @@
       <c r="J8" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K8" s="27" t="s">
+      <c r="K8" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="L8" s="27" t="s">
+      <c r="L8" s="22" t="s">
         <v>109</v>
       </c>
       <c r="M8" s="24"/>
@@ -1212,30 +1212,30 @@
       <c r="O8" s="13"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B9" s="27"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="35"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="28"/>
       <c r="I9" s="11" t="s">
         <v>39</v>
       </c>
       <c r="J9" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K9" s="27"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="26"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="25"/>
       <c r="N9" s="8"/>
       <c r="O9" s="13"/>
     </row>
     <row r="10" spans="2:15" ht="28" x14ac:dyDescent="0.3">
-      <c r="B10" s="27">
+      <c r="B10" s="22">
         <v>5</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="26" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="12" t="s">
@@ -1247,7 +1247,7 @@
       <c r="F10" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="G10" s="33" t="s">
+      <c r="G10" s="27" t="s">
         <v>136</v>
       </c>
       <c r="H10" s="11" t="s">
@@ -1257,7 +1257,7 @@
       <c r="J10" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K10" s="27" t="s">
+      <c r="K10" s="22" t="s">
         <v>1</v>
       </c>
       <c r="L10" s="11" t="s">
@@ -1272,8 +1272,8 @@
       <c r="O10" s="13"/>
     </row>
     <row r="11" spans="2:15" ht="28" x14ac:dyDescent="0.3">
-      <c r="B11" s="27"/>
-      <c r="C11" s="22"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="26"/>
       <c r="D11" s="12" t="s">
         <v>34</v>
       </c>
@@ -1283,7 +1283,7 @@
       <c r="F11" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="34"/>
+      <c r="G11" s="29"/>
       <c r="H11" s="11" t="s">
         <v>133</v>
       </c>
@@ -1291,7 +1291,7 @@
       <c r="J11" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K11" s="27"/>
+      <c r="K11" s="22"/>
       <c r="L11" s="11" t="s">
         <v>109</v>
       </c>
@@ -1304,8 +1304,8 @@
       <c r="O11" s="13"/>
     </row>
     <row r="12" spans="2:15" ht="28" x14ac:dyDescent="0.3">
-      <c r="B12" s="27"/>
-      <c r="C12" s="22"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="26"/>
       <c r="D12" s="12" t="s">
         <v>35</v>
       </c>
@@ -1315,7 +1315,7 @@
       <c r="F12" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="G12" s="34"/>
+      <c r="G12" s="29"/>
       <c r="H12" s="11" t="s">
         <v>133</v>
       </c>
@@ -1323,7 +1323,7 @@
       <c r="J12" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K12" s="27"/>
+      <c r="K12" s="22"/>
       <c r="L12" s="11" t="s">
         <v>109</v>
       </c>
@@ -1336,8 +1336,8 @@
       <c r="O12" s="13"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B13" s="27"/>
-      <c r="C13" s="22"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="26"/>
       <c r="D13" s="12" t="s">
         <v>43</v>
       </c>
@@ -1347,8 +1347,8 @@
       <c r="F13" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="G13" s="34"/>
-      <c r="H13" s="33" t="s">
+      <c r="G13" s="29"/>
+      <c r="H13" s="27" t="s">
         <v>134</v>
       </c>
       <c r="I13" s="11" t="s">
@@ -1357,7 +1357,7 @@
       <c r="J13" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K13" s="27"/>
+      <c r="K13" s="22"/>
       <c r="L13" s="11" t="s">
         <v>109</v>
       </c>
@@ -1366,8 +1366,8 @@
       <c r="O13" s="13"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B14" s="27"/>
-      <c r="C14" s="22"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="26"/>
       <c r="D14" s="20" t="s">
         <v>46</v>
       </c>
@@ -1377,15 +1377,15 @@
       <c r="F14" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
       <c r="I14" s="11" t="s">
         <v>117</v>
       </c>
       <c r="J14" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K14" s="27"/>
+      <c r="K14" s="22"/>
       <c r="L14" s="11" t="s">
         <v>109</v>
       </c>
@@ -1394,8 +1394,8 @@
       <c r="O14" s="13"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B15" s="27"/>
-      <c r="C15" s="22"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="26"/>
       <c r="D15" s="12" t="s">
         <v>48</v>
       </c>
@@ -1405,15 +1405,15 @@
       <c r="F15" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
       <c r="I15" s="11" t="s">
         <v>117</v>
       </c>
       <c r="J15" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K15" s="27"/>
+      <c r="K15" s="22"/>
       <c r="L15" s="11" t="s">
         <v>109</v>
       </c>
@@ -1422,8 +1422,8 @@
       <c r="O15" s="13"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B16" s="27"/>
-      <c r="C16" s="22"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="26"/>
       <c r="D16" s="12" t="s">
         <v>49</v>
       </c>
@@ -1433,15 +1433,15 @@
       <c r="F16" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
       <c r="I16" s="11" t="s">
         <v>117</v>
       </c>
       <c r="J16" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K16" s="27"/>
+      <c r="K16" s="22"/>
       <c r="L16" s="11" t="s">
         <v>109</v>
       </c>
@@ -1450,8 +1450,8 @@
       <c r="O16" s="13"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B17" s="27"/>
-      <c r="C17" s="22"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="26"/>
       <c r="D17" s="12" t="s">
         <v>50</v>
       </c>
@@ -1461,15 +1461,15 @@
       <c r="F17" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
       <c r="I17" s="11" t="s">
         <v>117</v>
       </c>
       <c r="J17" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K17" s="27"/>
+      <c r="K17" s="22"/>
       <c r="L17" s="11" t="s">
         <v>109</v>
       </c>
@@ -1598,10 +1598,10 @@
       <c r="O20" s="13"/>
     </row>
     <row r="21" spans="2:15" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="28">
+      <c r="B21" s="35">
         <v>9</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="C21" s="21" t="s">
         <v>19</v>
       </c>
       <c r="D21" s="13" t="s">
@@ -1623,7 +1623,7 @@
       <c r="J21" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="K21" s="27" t="s">
+      <c r="K21" s="22" t="s">
         <v>9</v>
       </c>
       <c r="L21" s="11" t="s">
@@ -1638,8 +1638,8 @@
       </c>
     </row>
     <row r="22" spans="2:15" ht="28" x14ac:dyDescent="0.3">
-      <c r="B22" s="28"/>
-      <c r="C22" s="23"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="21"/>
       <c r="D22" s="13" t="s">
         <v>68</v>
       </c>
@@ -1659,7 +1659,7 @@
       <c r="J22" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="K22" s="27"/>
+      <c r="K22" s="22"/>
       <c r="L22" s="11" t="s">
         <v>128</v>
       </c>
@@ -1672,8 +1672,8 @@
       </c>
     </row>
     <row r="23" spans="2:15" ht="28" x14ac:dyDescent="0.3">
-      <c r="B23" s="28"/>
-      <c r="C23" s="23"/>
+      <c r="B23" s="35"/>
+      <c r="C23" s="21"/>
       <c r="D23" s="13" t="s">
         <v>71</v>
       </c>
@@ -1693,7 +1693,7 @@
       <c r="J23" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="K23" s="27"/>
+      <c r="K23" s="22"/>
       <c r="L23" s="11" t="s">
         <v>128</v>
       </c>
@@ -1706,8 +1706,8 @@
       </c>
     </row>
     <row r="24" spans="2:15" ht="28" x14ac:dyDescent="0.3">
-      <c r="B24" s="28"/>
-      <c r="C24" s="23"/>
+      <c r="B24" s="35"/>
+      <c r="C24" s="21"/>
       <c r="D24" s="13" t="s">
         <v>95</v>
       </c>
@@ -1727,7 +1727,7 @@
       <c r="J24" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="K24" s="27"/>
+      <c r="K24" s="22"/>
       <c r="L24" s="11" t="s">
         <v>128</v>
       </c>
@@ -1740,88 +1740,88 @@
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B25" s="27">
+      <c r="B25" s="22">
         <v>10</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="C25" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="22" t="s">
+      <c r="D25" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="E25" s="22" t="s">
+      <c r="E25" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="F25" s="27" t="s">
+      <c r="F25" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="G25" s="27" t="s">
+      <c r="G25" s="22" t="s">
         <v>140</v>
       </c>
-      <c r="H25" s="33" t="s">
+      <c r="H25" s="27" t="s">
         <v>138</v>
       </c>
       <c r="I25" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="J25" s="27" t="s">
+      <c r="J25" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="K25" s="27" t="s">
+      <c r="K25" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="L25" s="33" t="s">
+      <c r="L25" s="27" t="s">
         <v>109</v>
       </c>
       <c r="M25" s="24" t="s">
         <v>148</v>
       </c>
       <c r="N25" s="8"/>
-      <c r="O25" s="23" t="s">
+      <c r="O25" s="21" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B26" s="27"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="34"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="29"/>
       <c r="I26" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="J26" s="27"/>
-      <c r="K26" s="27"/>
-      <c r="L26" s="34"/>
-      <c r="M26" s="25"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="22"/>
+      <c r="L26" s="29"/>
+      <c r="M26" s="36"/>
       <c r="N26" s="8"/>
-      <c r="O26" s="23"/>
+      <c r="O26" s="21"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B27" s="27"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="35"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="28"/>
       <c r="I27" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="J27" s="27"/>
-      <c r="K27" s="27"/>
-      <c r="L27" s="35"/>
-      <c r="M27" s="26"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="28"/>
+      <c r="M27" s="25"/>
       <c r="N27" s="8"/>
-      <c r="O27" s="23"/>
+      <c r="O27" s="21"/>
     </row>
     <row r="28" spans="2:15" ht="42" x14ac:dyDescent="0.3">
-      <c r="B28" s="27">
+      <c r="B28" s="22">
         <v>11</v>
       </c>
-      <c r="C28" s="22" t="s">
+      <c r="C28" s="26" t="s">
         <v>102</v>
       </c>
       <c r="D28" s="12" t="s">
@@ -1843,7 +1843,7 @@
       <c r="J28" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="K28" s="27" t="s">
+      <c r="K28" s="22" t="s">
         <v>9</v>
       </c>
       <c r="L28" s="11" t="s">
@@ -1858,8 +1858,8 @@
       </c>
     </row>
     <row r="29" spans="2:15" ht="28" x14ac:dyDescent="0.3">
-      <c r="B29" s="27"/>
-      <c r="C29" s="22"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="26"/>
       <c r="D29" s="12" t="s">
         <v>77</v>
       </c>
@@ -1879,7 +1879,7 @@
       <c r="J29" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="K29" s="27"/>
+      <c r="K29" s="22"/>
       <c r="L29" s="11" t="s">
         <v>109</v>
       </c>
@@ -1892,8 +1892,8 @@
       </c>
     </row>
     <row r="30" spans="2:15" ht="28" x14ac:dyDescent="0.3">
-      <c r="B30" s="27"/>
-      <c r="C30" s="22"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="26"/>
       <c r="D30" s="12" t="s">
         <v>80</v>
       </c>
@@ -1913,7 +1913,7 @@
       <c r="J30" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="K30" s="27"/>
+      <c r="K30" s="22"/>
       <c r="L30" s="11" t="s">
         <v>109</v>
       </c>
@@ -1926,8 +1926,8 @@
       </c>
     </row>
     <row r="31" spans="2:15" ht="28" x14ac:dyDescent="0.3">
-      <c r="B31" s="27"/>
-      <c r="C31" s="22"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="26"/>
       <c r="D31" s="12" t="s">
         <v>83</v>
       </c>
@@ -1947,7 +1947,7 @@
       <c r="J31" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="K31" s="27"/>
+      <c r="K31" s="22"/>
       <c r="L31" s="11" t="s">
         <v>109</v>
       </c>
@@ -1960,8 +1960,8 @@
       </c>
     </row>
     <row r="32" spans="2:15" ht="28" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="27"/>
-      <c r="C32" s="22"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="26"/>
       <c r="D32" s="12" t="s">
         <v>86</v>
       </c>
@@ -1981,7 +1981,7 @@
       <c r="J32" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="K32" s="27"/>
+      <c r="K32" s="22"/>
       <c r="L32" s="11" t="s">
         <v>128</v>
       </c>
@@ -1990,8 +1990,8 @@
       <c r="O32" s="13"/>
     </row>
     <row r="33" spans="2:15" ht="28" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="27"/>
-      <c r="C33" s="22"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="26"/>
       <c r="D33" s="12" t="s">
         <v>89</v>
       </c>
@@ -2011,7 +2011,7 @@
       <c r="J33" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="K33" s="27"/>
+      <c r="K33" s="22"/>
       <c r="L33" s="11" t="s">
         <v>128</v>
       </c>
@@ -11191,24 +11191,16 @@
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="O25:O27"/>
-    <mergeCell ref="K28:K33"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="C25:C27"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="D25:D27"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B17"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="G10:G17"/>
-    <mergeCell ref="G25:G27"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="H13:H17"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="K10:K17"/>
     <mergeCell ref="C28:C33"/>
     <mergeCell ref="B28:B33"/>
     <mergeCell ref="K2:K3"/>
@@ -11225,28 +11217,36 @@
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="I2:I3"/>
+    <mergeCell ref="C25:C27"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B17"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="G10:G17"/>
+    <mergeCell ref="G25:G27"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="C10:C17"/>
+    <mergeCell ref="E25:E27"/>
+    <mergeCell ref="F25:F27"/>
+    <mergeCell ref="H25:H27"/>
+    <mergeCell ref="O25:O27"/>
+    <mergeCell ref="K28:K33"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="M8:M9"/>
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="L2:L3"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="C10:C17"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="K10:K17"/>
     <mergeCell ref="K21:K24"/>
     <mergeCell ref="K25:K27"/>
     <mergeCell ref="L25:L27"/>
-    <mergeCell ref="E25:E27"/>
-    <mergeCell ref="F25:F27"/>
-    <mergeCell ref="H25:H27"/>
     <mergeCell ref="M25:M27"/>
     <mergeCell ref="M2:M3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="H13:H17"/>
-    <mergeCell ref="H2:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -11258,10 +11258,10 @@
   <dimension ref="B2:O951"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="M21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -11284,66 +11284,66 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="23" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="31" t="s">
         <v>127</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="31"/>
-      <c r="G2" s="36" t="s">
+      <c r="F2" s="32"/>
+      <c r="G2" s="34" t="s">
         <v>131</v>
       </c>
       <c r="H2" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="I2" s="31" t="s">
+      <c r="I2" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="29" t="s">
+      <c r="J2" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="K2" s="29" t="s">
+      <c r="K2" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="L2" s="29" t="s">
+      <c r="L2" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="M2" s="21" t="s">
+      <c r="M2" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="N2" s="21" t="s">
+      <c r="N2" s="23" t="s">
         <v>156</v>
       </c>
-      <c r="O2" s="21" t="s">
+      <c r="O2" s="23" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="3" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
       <c r="E3" s="4" t="s">
         <v>20</v>
       </c>
       <c r="F3" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="36"/>
+      <c r="G3" s="34"/>
       <c r="H3" s="38"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
     </row>
     <row r="4" spans="2:15" ht="28" x14ac:dyDescent="0.3">
       <c r="B4" s="10">
@@ -11426,25 +11426,25 @@
       <c r="O5" s="7"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B6" s="27">
+      <c r="B6" s="22">
         <v>3</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="32" t="s">
+      <c r="F6" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="27" t="s">
+      <c r="G6" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="H6" s="33" t="s">
+      <c r="H6" s="27" t="s">
         <v>5</v>
       </c>
       <c r="I6" s="11" t="s">
@@ -11453,10 +11453,10 @@
       <c r="J6" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K6" s="27" t="s">
+      <c r="K6" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="L6" s="27" t="s">
+      <c r="L6" s="22" t="s">
         <v>109</v>
       </c>
       <c r="M6" s="24"/>
@@ -11464,45 +11464,45 @@
       <c r="O6" s="7"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B7" s="27"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="35"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="28"/>
       <c r="I7" s="11" t="s">
         <v>6</v>
       </c>
       <c r="J7" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
-      <c r="M7" s="26"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="25"/>
       <c r="N7" s="8"/>
       <c r="O7" s="7"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B8" s="27">
+      <c r="B8" s="22">
         <v>4</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="32" t="s">
+      <c r="F8" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="G8" s="27" t="s">
+      <c r="G8" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="H8" s="33" t="s">
+      <c r="H8" s="27" t="s">
         <v>5</v>
       </c>
       <c r="I8" s="11" t="s">
@@ -11511,10 +11511,10 @@
       <c r="J8" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K8" s="27" t="s">
+      <c r="K8" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="L8" s="27" t="s">
+      <c r="L8" s="22" t="s">
         <v>109</v>
       </c>
       <c r="M8" s="24"/>
@@ -11522,30 +11522,30 @@
       <c r="O8" s="7"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B9" s="27"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="35"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="28"/>
       <c r="I9" s="11" t="s">
         <v>39</v>
       </c>
       <c r="J9" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K9" s="27"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="26"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="25"/>
       <c r="N9" s="8"/>
       <c r="O9" s="7"/>
     </row>
     <row r="10" spans="2:15" ht="28" x14ac:dyDescent="0.3">
-      <c r="B10" s="27">
+      <c r="B10" s="22">
         <v>5</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="26" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="6" t="s">
@@ -11557,7 +11557,7 @@
       <c r="F10" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="G10" s="33" t="s">
+      <c r="G10" s="27" t="s">
         <v>136</v>
       </c>
       <c r="H10" s="11" t="s">
@@ -11567,7 +11567,7 @@
       <c r="J10" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K10" s="27" t="s">
+      <c r="K10" s="22" t="s">
         <v>1</v>
       </c>
       <c r="L10" s="11" t="s">
@@ -11582,8 +11582,8 @@
       <c r="O10" s="7"/>
     </row>
     <row r="11" spans="2:15" ht="28" x14ac:dyDescent="0.3">
-      <c r="B11" s="27"/>
-      <c r="C11" s="22"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="26"/>
       <c r="D11" s="6" t="s">
         <v>34</v>
       </c>
@@ -11593,7 +11593,7 @@
       <c r="F11" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="34"/>
+      <c r="G11" s="29"/>
       <c r="H11" s="11" t="s">
         <v>133</v>
       </c>
@@ -11601,7 +11601,7 @@
       <c r="J11" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K11" s="27"/>
+      <c r="K11" s="22"/>
       <c r="L11" s="11" t="s">
         <v>109</v>
       </c>
@@ -11614,8 +11614,8 @@
       <c r="O11" s="7"/>
     </row>
     <row r="12" spans="2:15" ht="28" x14ac:dyDescent="0.3">
-      <c r="B12" s="27"/>
-      <c r="C12" s="22"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="26"/>
       <c r="D12" s="6" t="s">
         <v>35</v>
       </c>
@@ -11625,7 +11625,7 @@
       <c r="F12" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="G12" s="34"/>
+      <c r="G12" s="29"/>
       <c r="H12" s="11" t="s">
         <v>133</v>
       </c>
@@ -11633,7 +11633,7 @@
       <c r="J12" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K12" s="27"/>
+      <c r="K12" s="22"/>
       <c r="L12" s="11" t="s">
         <v>109</v>
       </c>
@@ -11646,8 +11646,8 @@
       <c r="O12" s="7"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B13" s="27"/>
-      <c r="C13" s="22"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="26"/>
       <c r="D13" s="6" t="s">
         <v>43</v>
       </c>
@@ -11657,8 +11657,8 @@
       <c r="F13" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="G13" s="34"/>
-      <c r="H13" s="33" t="s">
+      <c r="G13" s="29"/>
+      <c r="H13" s="27" t="s">
         <v>134</v>
       </c>
       <c r="I13" s="11" t="s">
@@ -11667,7 +11667,7 @@
       <c r="J13" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K13" s="27"/>
+      <c r="K13" s="22"/>
       <c r="L13" s="11" t="s">
         <v>109</v>
       </c>
@@ -11676,8 +11676,8 @@
       <c r="O13" s="7"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B14" s="27"/>
-      <c r="C14" s="22"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="26"/>
       <c r="D14" s="20" t="s">
         <v>46</v>
       </c>
@@ -11687,15 +11687,15 @@
       <c r="F14" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
       <c r="I14" s="11" t="s">
         <v>117</v>
       </c>
       <c r="J14" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K14" s="27"/>
+      <c r="K14" s="22"/>
       <c r="L14" s="11" t="s">
         <v>109</v>
       </c>
@@ -11704,8 +11704,8 @@
       <c r="O14" s="7"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B15" s="27"/>
-      <c r="C15" s="22"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="26"/>
       <c r="D15" s="6" t="s">
         <v>48</v>
       </c>
@@ -11715,15 +11715,15 @@
       <c r="F15" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
       <c r="I15" s="11" t="s">
         <v>117</v>
       </c>
       <c r="J15" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K15" s="27"/>
+      <c r="K15" s="22"/>
       <c r="L15" s="11" t="s">
         <v>109</v>
       </c>
@@ -11732,8 +11732,8 @@
       <c r="O15" s="7"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B16" s="27"/>
-      <c r="C16" s="22"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="26"/>
       <c r="D16" s="6" t="s">
         <v>49</v>
       </c>
@@ -11743,15 +11743,15 @@
       <c r="F16" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
       <c r="I16" s="11" t="s">
         <v>117</v>
       </c>
       <c r="J16" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K16" s="27"/>
+      <c r="K16" s="22"/>
       <c r="L16" s="11" t="s">
         <v>109</v>
       </c>
@@ -11760,8 +11760,8 @@
       <c r="O16" s="7"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B17" s="27"/>
-      <c r="C17" s="22"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="26"/>
       <c r="D17" s="6" t="s">
         <v>50</v>
       </c>
@@ -11771,15 +11771,15 @@
       <c r="F17" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
       <c r="I17" s="11" t="s">
         <v>117</v>
       </c>
       <c r="J17" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K17" s="27"/>
+      <c r="K17" s="22"/>
       <c r="L17" s="11" t="s">
         <v>109</v>
       </c>
@@ -11908,10 +11908,10 @@
       <c r="O20" s="7"/>
     </row>
     <row r="21" spans="2:15" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="28">
+      <c r="B21" s="35">
         <v>9</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="C21" s="21" t="s">
         <v>19</v>
       </c>
       <c r="D21" s="7" t="s">
@@ -11933,7 +11933,7 @@
       <c r="J21" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="K21" s="27" t="s">
+      <c r="K21" s="22" t="s">
         <v>9</v>
       </c>
       <c r="L21" s="11" t="s">
@@ -11948,8 +11948,8 @@
       </c>
     </row>
     <row r="22" spans="2:15" ht="28" x14ac:dyDescent="0.3">
-      <c r="B22" s="28"/>
-      <c r="C22" s="23"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="21"/>
       <c r="D22" s="7" t="s">
         <v>68</v>
       </c>
@@ -11969,7 +11969,7 @@
       <c r="J22" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="K22" s="27"/>
+      <c r="K22" s="22"/>
       <c r="L22" s="11" t="s">
         <v>128</v>
       </c>
@@ -11982,8 +11982,8 @@
       </c>
     </row>
     <row r="23" spans="2:15" ht="28" x14ac:dyDescent="0.3">
-      <c r="B23" s="28"/>
-      <c r="C23" s="23"/>
+      <c r="B23" s="35"/>
+      <c r="C23" s="21"/>
       <c r="D23" s="7" t="s">
         <v>71</v>
       </c>
@@ -12003,7 +12003,7 @@
       <c r="J23" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="K23" s="27"/>
+      <c r="K23" s="22"/>
       <c r="L23" s="11" t="s">
         <v>128</v>
       </c>
@@ -12016,8 +12016,8 @@
       </c>
     </row>
     <row r="24" spans="2:15" ht="28" x14ac:dyDescent="0.3">
-      <c r="B24" s="28"/>
-      <c r="C24" s="23"/>
+      <c r="B24" s="35"/>
+      <c r="C24" s="21"/>
       <c r="D24" s="7" t="s">
         <v>95</v>
       </c>
@@ -12037,7 +12037,7 @@
       <c r="J24" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="K24" s="27"/>
+      <c r="K24" s="22"/>
       <c r="L24" s="11" t="s">
         <v>128</v>
       </c>
@@ -12050,88 +12050,88 @@
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B25" s="27">
+      <c r="B25" s="22">
         <v>10</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="C25" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="22" t="s">
+      <c r="D25" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="E25" s="22" t="s">
+      <c r="E25" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="F25" s="27" t="s">
+      <c r="F25" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="G25" s="27" t="s">
+      <c r="G25" s="22" t="s">
         <v>140</v>
       </c>
-      <c r="H25" s="33" t="s">
+      <c r="H25" s="27" t="s">
         <v>138</v>
       </c>
       <c r="I25" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="J25" s="27" t="s">
+      <c r="J25" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="K25" s="27" t="s">
+      <c r="K25" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="L25" s="33" t="s">
+      <c r="L25" s="27" t="s">
         <v>109</v>
       </c>
       <c r="M25" s="24" t="s">
         <v>148</v>
       </c>
       <c r="N25" s="8"/>
-      <c r="O25" s="23" t="s">
+      <c r="O25" s="21" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B26" s="27"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="34"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="29"/>
       <c r="I26" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="J26" s="27"/>
-      <c r="K26" s="27"/>
-      <c r="L26" s="34"/>
-      <c r="M26" s="25"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="22"/>
+      <c r="L26" s="29"/>
+      <c r="M26" s="36"/>
       <c r="N26" s="8"/>
-      <c r="O26" s="23"/>
+      <c r="O26" s="21"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B27" s="27"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="35"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="28"/>
       <c r="I27" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="J27" s="27"/>
-      <c r="K27" s="27"/>
-      <c r="L27" s="35"/>
-      <c r="M27" s="26"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="28"/>
+      <c r="M27" s="25"/>
       <c r="N27" s="8"/>
-      <c r="O27" s="23"/>
+      <c r="O27" s="21"/>
     </row>
     <row r="28" spans="2:15" ht="42" x14ac:dyDescent="0.3">
-      <c r="B28" s="27">
+      <c r="B28" s="22">
         <v>11</v>
       </c>
-      <c r="C28" s="22" t="s">
+      <c r="C28" s="26" t="s">
         <v>102</v>
       </c>
       <c r="D28" s="6" t="s">
@@ -12153,7 +12153,7 @@
       <c r="J28" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="K28" s="27" t="s">
+      <c r="K28" s="22" t="s">
         <v>9</v>
       </c>
       <c r="L28" s="11" t="s">
@@ -12168,8 +12168,8 @@
       </c>
     </row>
     <row r="29" spans="2:15" ht="28" x14ac:dyDescent="0.3">
-      <c r="B29" s="27"/>
-      <c r="C29" s="22"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="26"/>
       <c r="D29" s="6" t="s">
         <v>77</v>
       </c>
@@ -12189,7 +12189,7 @@
       <c r="J29" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="K29" s="27"/>
+      <c r="K29" s="22"/>
       <c r="L29" s="11" t="s">
         <v>109</v>
       </c>
@@ -12202,8 +12202,8 @@
       </c>
     </row>
     <row r="30" spans="2:15" ht="28" x14ac:dyDescent="0.3">
-      <c r="B30" s="27"/>
-      <c r="C30" s="22"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="26"/>
       <c r="D30" s="6" t="s">
         <v>80</v>
       </c>
@@ -12223,7 +12223,7 @@
       <c r="J30" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="K30" s="27"/>
+      <c r="K30" s="22"/>
       <c r="L30" s="11" t="s">
         <v>109</v>
       </c>
@@ -12236,8 +12236,8 @@
       </c>
     </row>
     <row r="31" spans="2:15" ht="28" x14ac:dyDescent="0.3">
-      <c r="B31" s="27"/>
-      <c r="C31" s="22"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="26"/>
       <c r="D31" s="6" t="s">
         <v>83</v>
       </c>
@@ -12257,7 +12257,7 @@
       <c r="J31" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="K31" s="27"/>
+      <c r="K31" s="22"/>
       <c r="L31" s="11" t="s">
         <v>109</v>
       </c>
@@ -12270,8 +12270,8 @@
       </c>
     </row>
     <row r="32" spans="2:15" ht="28" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="27"/>
-      <c r="C32" s="22"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="26"/>
       <c r="D32" s="6" t="s">
         <v>86</v>
       </c>
@@ -12291,7 +12291,7 @@
       <c r="J32" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="K32" s="27"/>
+      <c r="K32" s="22"/>
       <c r="L32" s="11" t="s">
         <v>128</v>
       </c>
@@ -12300,8 +12300,8 @@
       <c r="O32" s="7"/>
     </row>
     <row r="33" spans="2:15" ht="28" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="27"/>
-      <c r="C33" s="22"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="26"/>
       <c r="D33" s="6" t="s">
         <v>89</v>
       </c>
@@ -12321,7 +12321,7 @@
       <c r="J33" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="K33" s="27"/>
+      <c r="K33" s="22"/>
       <c r="L33" s="11" t="s">
         <v>128</v>
       </c>
@@ -21501,11 +21501,41 @@
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H13:H17"/>
+    <mergeCell ref="L25:L27"/>
+    <mergeCell ref="M25:M27"/>
+    <mergeCell ref="O25:O27"/>
+    <mergeCell ref="B28:B33"/>
+    <mergeCell ref="C28:C33"/>
+    <mergeCell ref="K28:K33"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="C25:C27"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="E25:E27"/>
+    <mergeCell ref="F25:F27"/>
+    <mergeCell ref="G25:G27"/>
+    <mergeCell ref="J25:J27"/>
+    <mergeCell ref="K25:K27"/>
+    <mergeCell ref="B10:B17"/>
+    <mergeCell ref="C10:C17"/>
+    <mergeCell ref="K10:K17"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="C21:C24"/>
+    <mergeCell ref="K21:K24"/>
+    <mergeCell ref="G10:G17"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
     <mergeCell ref="H25:H27"/>
     <mergeCell ref="O2:O3"/>
     <mergeCell ref="B2:B3"/>
@@ -21522,41 +21552,11 @@
     <mergeCell ref="N2:N3"/>
     <mergeCell ref="K6:K7"/>
     <mergeCell ref="L6:L7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="B10:B17"/>
-    <mergeCell ref="C10:C17"/>
-    <mergeCell ref="K10:K17"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="C21:C24"/>
-    <mergeCell ref="K21:K24"/>
-    <mergeCell ref="G10:G17"/>
-    <mergeCell ref="B28:B33"/>
-    <mergeCell ref="C28:C33"/>
-    <mergeCell ref="K28:K33"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="C25:C27"/>
-    <mergeCell ref="D25:D27"/>
-    <mergeCell ref="E25:E27"/>
-    <mergeCell ref="F25:F27"/>
-    <mergeCell ref="G25:G27"/>
-    <mergeCell ref="J25:J27"/>
-    <mergeCell ref="K25:K27"/>
-    <mergeCell ref="L25:L27"/>
-    <mergeCell ref="M25:M27"/>
-    <mergeCell ref="O25:O27"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H13:H17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>